<commit_message>
staging content changes (-robo-commit)
</commit_message>
<xml_diff>
--- a/pegasus/sites.v3/advocacy.code.org/public/data/2022_state_of_cs_data.xlsx
+++ b/pegasus/sites.v3/advocacy.code.org/public/data/2022_state_of_cs_data.xlsx
@@ -59524,7 +59524,7 @@
         <v>0.00386</v>
       </c>
       <c r="F4" s="128">
-        <v>0.48</v>
+        <v>0.05</v>
       </c>
       <c r="G4" s="128">
         <v>0.05</v>
@@ -59607,7 +59607,7 @@
         <v>0.02057</v>
       </c>
       <c r="F5" s="136">
-        <v>0.48</v>
+        <v>0.04</v>
       </c>
       <c r="G5" s="136">
         <v>0.04</v>
@@ -59682,7 +59682,7 @@
         <v>0.00117</v>
       </c>
       <c r="F6" s="136">
-        <v>0.58</v>
+        <v>0.01</v>
       </c>
       <c r="G6" s="136">
         <v>0.01</v>
@@ -59757,7 +59757,7 @@
         <v>0.00964</v>
       </c>
       <c r="F7" s="136">
-        <v>0.61</v>
+        <v>0.02</v>
       </c>
       <c r="G7" s="136">
         <v>0.02</v>
@@ -59832,7 +59832,7 @@
         <v>0.00398</v>
       </c>
       <c r="F8" s="136">
-        <v>0.39</v>
+        <v>0.04</v>
       </c>
       <c r="G8" s="136">
         <v>0.04</v>
@@ -59907,7 +59907,7 @@
         <v>0.00445</v>
       </c>
       <c r="F9" s="136">
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
       <c r="G9" s="136">
         <v>0.12</v>
@@ -59982,7 +59982,7 @@
         <v>0.00266</v>
       </c>
       <c r="F10" s="136">
-        <v>0.54</v>
+        <v>0.03</v>
       </c>
       <c r="G10" s="136">
         <v>0.03</v>
@@ -60057,7 +60057,7 @@
         <v>0.00103</v>
       </c>
       <c r="F11" s="136">
-        <v>0.51</v>
+        <v>0.05</v>
       </c>
       <c r="G11" s="136">
         <v>0.05</v>
@@ -60132,7 +60132,7 @@
         <v>4.7E-4</v>
       </c>
       <c r="F12" s="136">
-        <v>0.09</v>
+        <v>0.02</v>
       </c>
       <c r="G12" s="136">
         <v>0.02</v>
@@ -60207,7 +60207,7 @@
         <v>0.00134</v>
       </c>
       <c r="F13" s="136">
-        <v>0.44</v>
+        <v>0.05</v>
       </c>
       <c r="G13" s="136">
         <v>0.05</v>
@@ -60282,7 +60282,7 @@
         <v>0.00166</v>
       </c>
       <c r="F14" s="136">
-        <v>0.38</v>
+        <v>0.03</v>
       </c>
       <c r="G14" s="136">
         <v>0.03</v>
@@ -60357,7 +60357,7 @@
         <v>0.0011</v>
       </c>
       <c r="F15" s="136">
-        <v>0.39</v>
+        <v>0.04</v>
       </c>
       <c r="G15" s="136">
         <v>0.04</v>
@@ -60432,7 +60432,7 @@
         <v>0.31404</v>
       </c>
       <c r="F16" s="136">
-        <v>0.12</v>
+        <v>0.31</v>
       </c>
       <c r="G16" s="136">
         <v>0.31</v>
@@ -60507,7 +60507,7 @@
         <v>0.0033</v>
       </c>
       <c r="F17" s="136">
-        <v>0.76</v>
+        <v>0.02</v>
       </c>
       <c r="G17" s="136">
         <v>0.02</v>
@@ -60582,7 +60582,7 @@
         <v>0.00296</v>
       </c>
       <c r="F18" s="136">
-        <v>0.76</v>
+        <v>0.01</v>
       </c>
       <c r="G18" s="136">
         <v>0.01</v>
@@ -60657,7 +60657,7 @@
         <v>0.00108</v>
       </c>
       <c r="F19" s="136">
-        <v>0.48</v>
+        <v>0.05</v>
       </c>
       <c r="G19" s="136">
         <v>0.05</v>
@@ -60732,7 +60732,7 @@
         <v>8.9E-4</v>
       </c>
       <c r="F20" s="136">
-        <v>0.67</v>
+        <v>0.02</v>
       </c>
       <c r="G20" s="136">
         <v>0.02</v>
@@ -60807,7 +60807,7 @@
         <v>0.00189</v>
       </c>
       <c r="F21" s="136">
-        <v>0.65</v>
+        <v>0.03</v>
       </c>
       <c r="G21" s="136">
         <v>0.03</v>
@@ -60882,7 +60882,7 @@
         <v>0.00126</v>
       </c>
       <c r="F22" s="136">
-        <v>0.76</v>
+        <v>0.02</v>
       </c>
       <c r="G22" s="136">
         <v>0.02</v>
@@ -60957,7 +60957,7 @@
         <v>8.0E-4</v>
       </c>
       <c r="F23" s="136">
-        <v>0.48</v>
+        <v>0.02</v>
       </c>
       <c r="G23" s="136">
         <v>0.02</v>
@@ -61032,7 +61032,7 @@
         <v>9.4E-4</v>
       </c>
       <c r="F24" s="136">
-        <v>0.57</v>
+        <v>0.07</v>
       </c>
       <c r="G24" s="136">
         <v>0.07</v>
@@ -61107,7 +61107,7 @@
         <v>0.00142</v>
       </c>
       <c r="F25" s="136">
-        <v>0.36</v>
+        <v>0.07</v>
       </c>
       <c r="G25" s="136">
         <v>0.07</v>
@@ -61182,7 +61182,7 @@
         <v>6.5E-4</v>
       </c>
       <c r="F26" s="136">
-        <v>0.89</v>
+        <v>0.02</v>
       </c>
       <c r="G26" s="136">
         <v>0.02</v>
@@ -61257,7 +61257,7 @@
         <v>8.7E-4</v>
       </c>
       <c r="F27" s="136">
-        <v>0.67</v>
+        <v>0.03</v>
       </c>
       <c r="G27" s="136">
         <v>0.03</v>
@@ -61332,7 +61332,7 @@
         <v>8.7E-4</v>
       </c>
       <c r="F28" s="136">
-        <v>0.66</v>
+        <v>0.06</v>
       </c>
       <c r="G28" s="136">
         <v>0.06</v>
@@ -61407,7 +61407,7 @@
         <v>0.00299</v>
       </c>
       <c r="F29" s="136">
-        <v>0.72</v>
+        <v>0.02</v>
       </c>
       <c r="G29" s="136">
         <v>0.02</v>
@@ -61482,7 +61482,7 @@
         <v>5.2E-4</v>
       </c>
       <c r="F30" s="136">
-        <v>0.48</v>
+        <v>0.01</v>
       </c>
       <c r="G30" s="136">
         <v>0.01</v>
@@ -61557,7 +61557,7 @@
         <v>0.00251</v>
       </c>
       <c r="F31" s="136">
-        <v>0.78</v>
+        <v>0.01</v>
       </c>
       <c r="G31" s="136">
         <v>0.01</v>
@@ -61632,7 +61632,7 @@
         <v>0.00121</v>
       </c>
       <c r="F32" s="136">
-        <v>0.49</v>
+        <v>0.03</v>
       </c>
       <c r="G32" s="136">
         <v>0.03</v>
@@ -61707,7 +61707,7 @@
         <v>0.00217</v>
       </c>
       <c r="F33" s="136">
-        <v>0.74</v>
+        <v>0.01</v>
       </c>
       <c r="G33" s="136">
         <v>0.01</v>
@@ -61782,7 +61782,7 @@
         <v>0.00144</v>
       </c>
       <c r="F34" s="136">
-        <v>0.67</v>
+        <v>0.03</v>
       </c>
       <c r="G34" s="136">
         <v>0.03</v>
@@ -61857,7 +61857,7 @@
         <v>9.1E-4</v>
       </c>
       <c r="F35" s="136">
-        <v>0.85</v>
+        <v>0.03</v>
       </c>
       <c r="G35" s="136">
         <v>0.03</v>
@@ -61932,7 +61932,7 @@
         <v>0.00203</v>
       </c>
       <c r="F36" s="136">
-        <v>0.41</v>
+        <v>0.1</v>
       </c>
       <c r="G36" s="136">
         <v>0.1</v>
@@ -62007,7 +62007,7 @@
         <v>0.00133</v>
       </c>
       <c r="F37" s="136">
-        <v>0.22</v>
+        <v>0.01</v>
       </c>
       <c r="G37" s="136">
         <v>0.01</v>
@@ -62082,7 +62082,7 @@
         <v>0.01537</v>
       </c>
       <c r="F38" s="136">
-        <v>0.31</v>
+        <v>0.06</v>
       </c>
       <c r="G38" s="136">
         <v>0.06</v>
@@ -62157,7 +62157,7 @@
         <v>0.00274</v>
       </c>
       <c r="F39" s="136">
-        <v>0.42</v>
+        <v>0.09</v>
       </c>
       <c r="G39" s="136">
         <v>0.09</v>
@@ -62232,7 +62232,7 @@
         <v>9.5E-4</v>
       </c>
       <c r="F40" s="136">
-        <v>0.68</v>
+        <v>0.02</v>
       </c>
       <c r="G40" s="136">
         <v>0.02</v>
@@ -62307,7 +62307,7 @@
         <v>0.00356</v>
       </c>
       <c r="F41" s="136">
-        <v>0.49</v>
+        <v>0.02</v>
       </c>
       <c r="G41" s="136">
         <v>0.02</v>
@@ -62382,7 +62382,7 @@
         <v>0.00724</v>
       </c>
       <c r="F42" s="136">
-        <v>0.63</v>
+        <v>0.04</v>
       </c>
       <c r="G42" s="136">
         <v>0.04</v>
@@ -62457,7 +62457,7 @@
         <v>9.2E-4</v>
       </c>
       <c r="F43" s="136">
-        <v>0.65</v>
+        <v>0.04</v>
       </c>
       <c r="G43" s="136">
         <v>0.04</v>
@@ -62532,7 +62532,7 @@
         <v>0.00155</v>
       </c>
       <c r="F44" s="136">
-        <v>0.56</v>
+        <v>0.03</v>
       </c>
       <c r="G44" s="136">
         <v>0.03</v>
@@ -62607,7 +62607,7 @@
         <v>0.00138</v>
       </c>
       <c r="F45" s="136">
-        <v>0.52</v>
+        <v>0.02</v>
       </c>
       <c r="G45" s="136">
         <v>0.02</v>
@@ -62682,7 +62682,7 @@
         <v>0.00105</v>
       </c>
       <c r="F46" s="136">
-        <v>0.68</v>
+        <v>0.02</v>
       </c>
       <c r="G46" s="136">
         <v>0.02</v>
@@ -62757,7 +62757,7 @@
         <v>0.00103</v>
       </c>
       <c r="F47" s="136">
-        <v>0.63</v>
+        <v>0.02</v>
       </c>
       <c r="G47" s="136">
         <v>0.02</v>
@@ -62832,7 +62832,7 @@
         <v>0.0015</v>
       </c>
       <c r="F48" s="136">
-        <v>0.28</v>
+        <v>0.05</v>
       </c>
       <c r="G48" s="136">
         <v>0.05</v>
@@ -62907,7 +62907,7 @@
         <v>0.01526</v>
       </c>
       <c r="F49" s="136">
-        <v>0.74</v>
+        <v>0.02</v>
       </c>
       <c r="G49" s="136">
         <v>0.02</v>
@@ -62982,7 +62982,7 @@
         <v>0.00169</v>
       </c>
       <c r="F50" s="136">
-        <v>0.49</v>
+        <v>0.08</v>
       </c>
       <c r="G50" s="136">
         <v>0.08</v>
@@ -63057,7 +63057,7 @@
         <v>0.00157</v>
       </c>
       <c r="F51" s="136">
-        <v>0.89</v>
+        <v>0.02</v>
       </c>
       <c r="G51" s="136">
         <v>0.02</v>
@@ -63132,7 +63132,7 @@
         <v>0.01171</v>
       </c>
       <c r="F52" s="136">
-        <v>0.54</v>
+        <v>0.08</v>
       </c>
       <c r="G52" s="136">
         <v>0.08</v>
@@ -63207,7 +63207,7 @@
         <v>7.5E-4</v>
       </c>
       <c r="F53" s="136">
-        <v>0.7</v>
+        <v>0.04</v>
       </c>
       <c r="G53" s="136">
         <v>0.04</v>
@@ -63282,7 +63282,7 @@
         <v>5.4E-4</v>
       </c>
       <c r="F54" s="136">
-        <v>0.9</v>
+        <v>0.01</v>
       </c>
       <c r="G54" s="136">
         <v>0.01</v>
@@ -63357,7 +63357,7 @@
         <v>0.00154</v>
       </c>
       <c r="F55" s="136">
-        <v>0.78</v>
+        <v>0.01</v>
       </c>
       <c r="G55" s="136">
         <v>0.01</v>

</xml_diff>